<commit_message>
Realizando 4, 5, 6
</commit_message>
<xml_diff>
--- a/Net_switching/estadisticas.xlsx
+++ b/Net_switching/estadisticas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Ortega\Documents\GitHub\collado_ortega_telematics\Net_switching\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBEFA85-611C-4535-8DED-A69DAC5E3CF2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358E49B0-E484-4A8D-9E8C-2718920A6E8C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BDA7FA0A-50C1-4A7A-B6BA-B251FAF47C00}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Lower Limit</t>
   </si>
@@ -91,6 +91,53 @@
   </si>
   <si>
     <t>Comprobación</t>
+  </si>
+  <si>
+    <t>Cálculos</t>
+  </si>
+  <si>
+    <r>
+      <t>1/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>λ</t>
+    </r>
+  </si>
+  <si>
+    <t>λ</t>
+  </si>
+  <si>
+    <t>Lpa</t>
+  </si>
+  <si>
+    <t>Lpb</t>
+  </si>
+  <si>
+    <t>Rb</t>
+  </si>
+  <si>
+    <t>μa</t>
+  </si>
+  <si>
+    <t>1/μa</t>
+  </si>
+  <si>
+    <t>1/μb</t>
+  </si>
+  <si>
+    <t>μb</t>
+  </si>
+  <si>
+    <t>ρa</t>
+  </si>
+  <si>
+    <t>ρb</t>
   </si>
 </sst>
 </file>
@@ -100,7 +147,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +162,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -148,10 +201,17 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,13 +537,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{405B9B6D-A717-4B65-ACAB-44AF15A21D56}">
-  <dimension ref="B3:K27"/>
+  <dimension ref="B3:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
@@ -492,11 +556,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
       <c r="K3" s="1" t="s">
         <v>19</v>
       </c>
@@ -546,7 +610,7 @@
         <f>C5-D5</f>
         <v>9.2644459999999956E-3</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="6">
         <f>G5/C5</f>
         <v>0.1438991946444243</v>
       </c>
@@ -571,7 +635,7 @@
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" ref="G7:G27" si="0">(E7-D7)/2</f>
+        <f t="shared" ref="G7:G33" si="0">(E7-D7)/2</f>
         <v>0</v>
       </c>
       <c r="H7" s="3">
@@ -579,11 +643,11 @@
         <v>0</v>
       </c>
       <c r="I7" s="3">
-        <f t="shared" ref="I7:I27" si="1">C7-D7</f>
+        <f t="shared" ref="I7:I33" si="1">C7-D7</f>
         <v>0</v>
       </c>
       <c r="K7" s="4">
-        <f t="shared" ref="K6:K27" si="2">G7/C7</f>
+        <f t="shared" ref="K7:K33" si="2">G7/C7</f>
         <v>0</v>
       </c>
     </row>
@@ -618,7 +682,7 @@
         <f t="shared" si="1"/>
         <v>5.8212528999999957E-2</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="6">
         <f t="shared" si="2"/>
         <v>0.163099155358191</v>
       </c>
@@ -654,7 +718,7 @@
         <f t="shared" si="1"/>
         <v>5.5579069999999939E-3</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="6">
         <f t="shared" si="2"/>
         <v>8.6327702833888589E-2</v>
       </c>
@@ -726,7 +790,7 @@
         <f t="shared" si="1"/>
         <v>3.492273899999998E-2</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K15" s="6">
         <f t="shared" si="2"/>
         <v>9.7846106552837334E-2</v>
       </c>
@@ -765,7 +829,7 @@
         <f t="shared" si="1"/>
         <v>5.450272000000006E-3</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K17" s="6">
         <f t="shared" si="2"/>
         <v>9.5543460103945085E-2</v>
       </c>
@@ -837,7 +901,7 @@
         <f t="shared" si="1"/>
         <v>3.3518763000000007E-2</v>
       </c>
-      <c r="K21" s="7">
+      <c r="K21" s="6">
         <f t="shared" si="2"/>
         <v>0.10766930982416938</v>
       </c>
@@ -876,7 +940,7 @@
         <f t="shared" si="1"/>
         <v>3.8125369999999978E-3</v>
       </c>
-      <c r="K23" s="7">
+      <c r="K23" s="6">
         <f t="shared" si="2"/>
         <v>6.6412524765095723E-2</v>
       </c>
@@ -948,16 +1012,351 @@
         <f t="shared" si="1"/>
         <v>2.1110722999999998E-2</v>
       </c>
-      <c r="K27" s="7">
+      <c r="K27" s="6">
         <f t="shared" si="2"/>
         <v>6.8629550445806639E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="K28" s="6"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="3">
+        <v>2.8703453E-2</v>
+      </c>
+      <c r="D29" s="3">
+        <v>2.6797184000000002E-2</v>
+      </c>
+      <c r="E29" s="3">
+        <v>3.0609721999999999E-2</v>
+      </c>
+      <c r="G29" s="3">
+        <f t="shared" si="0"/>
+        <v>1.9062689999999986E-3</v>
+      </c>
+      <c r="H29" s="3">
+        <f t="shared" ref="H28:H33" si="3">(E29-D29)/2</f>
+        <v>1.9062689999999986E-3</v>
+      </c>
+      <c r="I29" s="3">
+        <f t="shared" si="1"/>
+        <v>1.9062689999999986E-3</v>
+      </c>
+      <c r="K29" s="6">
+        <f t="shared" si="2"/>
+        <v>6.6412532317975767E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="K30" s="6"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="3">
+        <v>6.2500000000000003E-3</v>
+      </c>
+      <c r="D31" s="3">
+        <v>6.2500000000000003E-3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>6.2500000000000003E-3</v>
+      </c>
+      <c r="G31" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="K32" s="6"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0.27708160799999998</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0.25847334700000002</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0.29568986899999999</v>
+      </c>
+      <c r="G33" s="3">
+        <f t="shared" si="0"/>
+        <v>1.8608260999999987E-2</v>
+      </c>
+      <c r="H33" s="3">
+        <f t="shared" si="3"/>
+        <v>1.8608260999999987E-2</v>
+      </c>
+      <c r="I33" s="3">
+        <f t="shared" si="1"/>
+        <v>1.8608260999999959E-2</v>
+      </c>
+      <c r="K33" s="6">
+        <f t="shared" si="2"/>
+        <v>6.7158051861746046E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C38" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C39" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>0.5</v>
+      </c>
+      <c r="D40">
+        <f>1/C40</f>
+        <v>2</v>
+      </c>
+      <c r="E40" s="2">
+        <f>D40*$D$52</f>
+        <v>0.125</v>
+      </c>
+      <c r="F40" s="2">
+        <f>D40*$D$54</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <f t="shared" ref="D41:D46" si="4">1/C41</f>
+        <v>1</v>
+      </c>
+      <c r="E41" s="2">
+        <f>D41*$D$52</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F41" s="2">
+        <f>D41*$D$54</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="E42" s="2">
+        <f>D42*$D$52</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F42" s="2">
+        <f>D42*$D$54</f>
+        <v>6.2500000000000003E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="4"/>
+        <v>0.25</v>
+      </c>
+      <c r="E43" s="2">
+        <f>D43*$D$52</f>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="F43" s="2">
+        <f>D43*$D$54</f>
+        <v>3.1250000000000002E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <v>6</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="4"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E44" s="2">
+        <f>D44*$D$52</f>
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="F44" s="2">
+        <f>D44*$D$54</f>
+        <v>2.0833333333333333E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>6</v>
+      </c>
+      <c r="C45">
+        <v>8</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="4"/>
+        <v>0.125</v>
+      </c>
+      <c r="E45" s="2">
+        <f>D45*$D$52</f>
+        <v>7.8125E-3</v>
+      </c>
+      <c r="F45" s="2">
+        <f>D45*$D$54</f>
+        <v>1.5625000000000001E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>7</v>
+      </c>
+      <c r="C46">
+        <v>10</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="4"/>
+        <v>0.1</v>
+      </c>
+      <c r="E46" s="2">
+        <f>D46*$D$52</f>
+        <v>6.2500000000000003E-3</v>
+      </c>
+      <c r="F46" s="2">
+        <f>D46*$D$54</f>
+        <v>1.2500000000000002E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48">
+        <f>1000*8</f>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>24</v>
+      </c>
+      <c r="D49">
+        <f>200*8</f>
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>25</v>
+      </c>
+      <c r="D50">
+        <v>128000</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C52" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D52">
+        <f>D48/D50</f>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>26</v>
+      </c>
+      <c r="D53">
+        <f>1/D52</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C54" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D54">
+        <f>D49/D50</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>29</v>
+      </c>
+      <c r="D55">
+        <f>1/D54</f>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="G3:I3"/>
   </mergeCells>
-  <conditionalFormatting sqref="K5:K27">
+  <conditionalFormatting sqref="K5:K33">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>

</xml_diff>